<commit_message>
changing data transformation logic
</commit_message>
<xml_diff>
--- a/power_bi_input/input.xlsx
+++ b/power_bi_input/input.xlsx
@@ -54,7 +54,7 @@
     <t>Achieved</t>
   </si>
   <si>
-    <t>Not Achieved</t>
+    <t>NA</t>
   </si>
   <si>
     <t>Missing</t>
@@ -8127,7 +8127,7 @@
         <v>208</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H57">
         <v>0.4</v>
@@ -8153,7 +8153,7 @@
         <v>208</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H58">
         <v>0.4</v>
@@ -8179,7 +8179,7 @@
         <v>236</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H59">
         <v>0.4</v>
@@ -8205,7 +8205,7 @@
         <v>237</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H60">
         <v>0.4</v>
@@ -8231,7 +8231,7 @@
         <v>237</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H61">
         <v>0.4</v>
@@ -8257,7 +8257,7 @@
         <v>208</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H62">
         <v>0.4</v>
@@ -8283,7 +8283,7 @@
         <v>208</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H63">
         <v>0.4</v>
@@ -8309,7 +8309,7 @@
         <v>208</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H64">
         <v>0.4</v>
@@ -8335,7 +8335,7 @@
         <v>208</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H65">
         <v>0.4</v>
@@ -8361,7 +8361,7 @@
         <v>208</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H66">
         <v>0.4</v>
@@ -8387,7 +8387,7 @@
         <v>238</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H67">
         <v>0.4</v>
@@ -8413,7 +8413,7 @@
         <v>239</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H68">
         <v>0.4</v>
@@ -8439,7 +8439,7 @@
         <v>208</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H69">
         <v>0.4</v>
@@ -8465,7 +8465,7 @@
         <v>208</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H70">
         <v>0.4</v>
@@ -8491,7 +8491,7 @@
         <v>208</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H71">
         <v>0.4</v>
@@ -8517,7 +8517,7 @@
         <v>240</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H72">
         <v>0.4</v>
@@ -8543,7 +8543,7 @@
         <v>213</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H73">
         <v>0.4</v>
@@ -8569,7 +8569,7 @@
         <v>241</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H74">
         <v>0.4</v>
@@ -8595,7 +8595,7 @@
         <v>242</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H75">
         <v>0.4</v>
@@ -8621,7 +8621,7 @@
         <v>242</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H76">
         <v>0.4</v>
@@ -8647,7 +8647,7 @@
         <v>208</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H77">
         <v>0.4</v>
@@ -8673,7 +8673,7 @@
         <v>208</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H78">
         <v>0.4</v>
@@ -8699,7 +8699,7 @@
         <v>208</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H79">
         <v>0.4</v>
@@ -8725,7 +8725,7 @@
         <v>208</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H80">
         <v>0.4</v>
@@ -8751,7 +8751,7 @@
         <v>208</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H81">
         <v>0.4</v>
@@ -12417,7 +12417,7 @@
         <v>261</v>
       </c>
       <c r="G222">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H222">
         <v>1</v>
@@ -12443,7 +12443,7 @@
         <v>279</v>
       </c>
       <c r="G223">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H223">
         <v>1</v>
@@ -12469,7 +12469,7 @@
         <v>287</v>
       </c>
       <c r="G224">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H224">
         <v>1</v>
@@ -13665,7 +13665,7 @@
         <v>208</v>
       </c>
       <c r="G270">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H270">
         <v>0.5</v>
@@ -13691,7 +13691,7 @@
         <v>208</v>
       </c>
       <c r="G271">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H271">
         <v>0.5</v>
@@ -13717,7 +13717,7 @@
         <v>208</v>
       </c>
       <c r="G272">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H272">
         <v>0.5</v>
@@ -13743,7 +13743,7 @@
         <v>208</v>
       </c>
       <c r="G273">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H273">
         <v>0.5</v>
@@ -13769,7 +13769,7 @@
         <v>208</v>
       </c>
       <c r="G274">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H274">
         <v>0</v>
@@ -13795,7 +13795,7 @@
         <v>238</v>
       </c>
       <c r="G275">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H275">
         <v>0.5</v>
@@ -13821,7 +13821,7 @@
         <v>238</v>
       </c>
       <c r="G276">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H276">
         <v>0.5</v>
@@ -13847,7 +13847,7 @@
         <v>240</v>
       </c>
       <c r="G277">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H277">
         <v>0.5</v>
@@ -13873,7 +13873,7 @@
         <v>299</v>
       </c>
       <c r="G278">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H278">
         <v>0.5</v>
@@ -13899,7 +13899,7 @@
         <v>208</v>
       </c>
       <c r="G279">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H279">
         <v>0</v>

</xml_diff>